<commit_message>
Changed success feedback response
</commit_message>
<xml_diff>
--- a/src/private/templates/success_feedback_responses.xlsx
+++ b/src/private/templates/success_feedback_responses.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="51200" windowHeight="28260" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17460" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,44 +35,54 @@
     <t>Supplier name</t>
   </si>
   <si>
-    <t>Employment before</t>
-  </si>
-  <si>
-    <t>Employment now</t>
-  </si>
-  <si>
-    <t>National spend before</t>
-  </si>
-  <si>
-    <t>National spend after</t>
-  </si>
-  <si>
-    <t>Investment / Capital</t>
-  </si>
-  <si>
-    <t>Trainings</t>
-  </si>
-  <si>
     <t>Corporate social responsibility</t>
   </si>
   <si>
-    <t>Technology improvement</t>
-  </si>
-  <si>
-    <t>Umnugobi spend before</t>
-  </si>
-  <si>
-    <t>Umnugobi spend now</t>
-  </si>
-  <si>
     <t>#</t>
+  </si>
+  <si>
+    <t>Total employment / National</t>
+  </si>
+  <si>
+    <t>Total employment / Umnugobi</t>
+  </si>
+  <si>
+    <t>Employee work related to scope / National</t>
+  </si>
+  <si>
+    <t>Procurement spend / Total</t>
+  </si>
+  <si>
+    <t>Procurement spend / National</t>
+  </si>
+  <si>
+    <t>Procurement spend / Umnugobi</t>
+  </si>
+  <si>
+    <t>Other stories to share</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Employee work related to scope / </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="0"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>Umnugobi</t>
+    </r>
+  </si>
+  <si>
+    <t>Total employment / changes</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -80,13 +90,39 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="0"/>
+      <name val="Calibri (Body)"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1" tint="0.34998626667073579"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -101,10 +137,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -385,85 +430,94 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="244" zoomScaleNormal="244" zoomScalePageLayoutView="244" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" zoomScale="109" zoomScaleNormal="109" zoomScalePageLayoutView="109" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="4.83203125" customWidth="1"/>
     <col min="2" max="2" width="21.6640625" customWidth="1"/>
-    <col min="4" max="4" width="20.33203125" customWidth="1"/>
-    <col min="5" max="5" width="29" customWidth="1"/>
-    <col min="6" max="6" width="20.5" customWidth="1"/>
-    <col min="7" max="10" width="21.5" customWidth="1"/>
-    <col min="12" max="12" width="24.83203125" customWidth="1"/>
-    <col min="13" max="13" width="20.83203125" customWidth="1"/>
+    <col min="4" max="5" width="17.33203125" customWidth="1"/>
+    <col min="6" max="6" width="18.5" customWidth="1"/>
+    <col min="7" max="7" width="17.33203125" customWidth="1"/>
+    <col min="8" max="8" width="16" customWidth="1"/>
+    <col min="9" max="9" width="16.83203125" customWidth="1"/>
+    <col min="10" max="11" width="21.5" customWidth="1"/>
+    <col min="12" max="12" width="36.5" customWidth="1"/>
+    <col min="13" max="13" width="40.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="C2" s="1" t="s">
+    <row r="2" spans="1:13" ht="32" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="4"/>
+      <c r="I2" s="4"/>
+      <c r="J2" s="4"/>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
+    <row r="3" spans="1:13" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+    <row r="4" spans="1:13" s="1" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C4" t="s">
-        <v>0</v>
-      </c>
-      <c r="D4" t="s">
+      <c r="G4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="L4" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E4" t="s">
-        <v>4</v>
-      </c>
-      <c r="F4" t="s">
-        <v>5</v>
-      </c>
-      <c r="G4" t="s">
-        <v>6</v>
-      </c>
-      <c r="H4" t="s">
+      <c r="M4" s="2" t="s">
         <v>11</v>
-      </c>
-      <c r="I4" t="s">
-        <v>12</v>
-      </c>
-      <c r="J4" t="s">
-        <v>7</v>
-      </c>
-      <c r="K4" t="s">
-        <v>8</v>
-      </c>
-      <c r="L4" t="s">
-        <v>9</v>
-      </c>
-      <c r="M4" t="s">
-        <v>10</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="C3:E3"/>
-    <mergeCell ref="C2:E2"/>
-    <mergeCell ref="C1:E1"/>
+    <mergeCell ref="C3:F3"/>
+    <mergeCell ref="C1:F1"/>
+    <mergeCell ref="C2:J2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>